<commit_message>
Minor updates to the code to improve ease of running
</commit_message>
<xml_diff>
--- a/prop_speed_algo_analysis.xlsx
+++ b/prop_speed_algo_analysis.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph Mockler\Documents\GitHub\2025_Hypersonic_BL_ID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FF1964-C4E2-42E4-8B8E-20D6CD37A25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5197F9C4-2D4F-4DE7-A2DE-80E91E6EEB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8D8D13B6-77FA-429E-A967-DF3D97238217}"/>
+    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="4" xr2:uid="{8D8D13B6-77FA-429E-A967-DF3D97238217}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="140">
   <si>
     <t>Means</t>
   </si>
@@ -418,12 +419,57 @@
   <si>
     <t>Pix trav interp</t>
   </si>
+  <si>
+    <t>run 33</t>
+  </si>
+  <si>
+    <t>run 34</t>
+  </si>
+  <si>
+    <t>run 38</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>2dc</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>2dw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">·       Re66 (Run 38): Ue </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 835.3/0.91 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">·       Re79 (Run34): Ue </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 824.9/0.90 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">·       Re97 (Run33): Ue </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 819.9/0.90 </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +486,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -449,7 +508,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -457,13 +516,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="6"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11674,7 +11855,7 @@
         <v>37.1</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13:AK13" si="2">D13+0.1</f>
+        <f t="shared" ref="O13:X13" si="2">D13+0.1</f>
         <v>38.1</v>
       </c>
       <c r="P13">
@@ -14354,8 +14535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A46BB33-BA68-4DAA-A4EC-DEF4264FFE96}">
   <dimension ref="C2:O684"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
-      <selection activeCell="F373" sqref="F373"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20178,4 +20359,267 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC38404-0143-4D9B-BE7A-21EE2248F503}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="4">
+        <v>818.09</v>
+      </c>
+      <c r="C2" s="5">
+        <v>834.55</v>
+      </c>
+      <c r="D2" s="5">
+        <v>829.72</v>
+      </c>
+      <c r="E2" s="6">
+        <v>819.2</v>
+      </c>
+      <c r="G2" s="13">
+        <f>B2/$D$11</f>
+        <v>0.89801317233809008</v>
+      </c>
+      <c r="H2" s="13">
+        <f t="shared" ref="H2:J2" si="0">C2/$D$11</f>
+        <v>0.91608122941822168</v>
+      </c>
+      <c r="I2" s="13">
+        <f t="shared" si="0"/>
+        <v>0.91077936333699239</v>
+      </c>
+      <c r="J2" s="13">
+        <f t="shared" si="0"/>
+        <v>0.89923161361141613</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="7">
+        <v>13.24</v>
+      </c>
+      <c r="C3" s="8">
+        <v>31.8</v>
+      </c>
+      <c r="D3" s="8">
+        <v>36.94</v>
+      </c>
+      <c r="E3" s="9">
+        <v>11.5</v>
+      </c>
+      <c r="G3" s="14">
+        <f>G2*(B3/B2)</f>
+        <v>1.4533479692645445E-2</v>
+      </c>
+      <c r="H3" s="14">
+        <f t="shared" ref="H3:J3" si="1">H2*(C3/C2)</f>
+        <v>3.4906695938529089E-2</v>
+      </c>
+      <c r="I3" s="14">
+        <f t="shared" si="1"/>
+        <v>4.0548847420417124E-2</v>
+      </c>
+      <c r="J3" s="14">
+        <f t="shared" si="1"/>
+        <v>1.2623490669593854E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="7">
+        <v>814.61</v>
+      </c>
+      <c r="C4" s="8">
+        <v>818.49</v>
+      </c>
+      <c r="D4" s="8">
+        <v>833.78</v>
+      </c>
+      <c r="E4" s="9">
+        <v>824.6</v>
+      </c>
+      <c r="G4" s="13">
+        <f>B4/$D$11</f>
+        <v>0.89419319429198685</v>
+      </c>
+      <c r="H4" s="13">
+        <f t="shared" ref="H4" si="2">C4/$D$11</f>
+        <v>0.89845225027442377</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" ref="I4" si="3">D4/$D$11</f>
+        <v>0.91523600439077935</v>
+      </c>
+      <c r="J4" s="13">
+        <f t="shared" ref="J4" si="4">E4/$D$11</f>
+        <v>0.90515916575192101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="7">
+        <v>11.54</v>
+      </c>
+      <c r="C5" s="8">
+        <v>22.17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>75.8</v>
+      </c>
+      <c r="E5" s="9">
+        <v>20.9</v>
+      </c>
+      <c r="G5" s="14">
+        <f>G4*(B5/B4)</f>
+        <v>1.2667398463227222E-2</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" ref="H5" si="5">H4*(C5/C4)</f>
+        <v>2.4335894621295283E-2</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" ref="I5" si="6">I4*(D5/D4)</f>
+        <v>8.3205268935235999E-2</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" ref="J5" si="7">J4*(E5/E4)</f>
+        <v>2.2941822173435784E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="7">
+        <v>828.54</v>
+      </c>
+      <c r="C6" s="8">
+        <v>849.12</v>
+      </c>
+      <c r="D6" s="8">
+        <v>838.76</v>
+      </c>
+      <c r="E6" s="9">
+        <v>835.3</v>
+      </c>
+      <c r="G6" s="13">
+        <f>B6/$D$11</f>
+        <v>0.90948408342480791</v>
+      </c>
+      <c r="H6" s="13">
+        <f t="shared" ref="H6" si="8">C6/$D$11</f>
+        <v>0.93207464324917677</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" ref="I6" si="9">D6/$D$11</f>
+        <v>0.92070252469813396</v>
+      </c>
+      <c r="J6" s="13">
+        <f t="shared" ref="J6" si="10">E6/$D$11</f>
+        <v>0.91690450054884742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="10">
+        <v>36.94</v>
+      </c>
+      <c r="C7" s="11">
+        <v>25.81</v>
+      </c>
+      <c r="D7" s="11">
+        <v>31.1</v>
+      </c>
+      <c r="E7" s="12">
+        <v>40.6</v>
+      </c>
+      <c r="G7" s="13">
+        <f>G6*(B7/B6)</f>
+        <v>4.0548847420417124E-2</v>
+      </c>
+      <c r="H7" s="13">
+        <f t="shared" ref="H7" si="11">H6*(C7/C6)</f>
+        <v>2.8331503841931942E-2</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" ref="I7" si="12">I6*(D7/D6)</f>
+        <v>3.4138309549945116E-2</v>
+      </c>
+      <c r="J7" s="13">
+        <f t="shared" ref="J7" si="13">J6*(E7/E6)</f>
+        <v>4.4566410537870471E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="3">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" s="3">
+        <v>916.55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="3">
+        <v>917.91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>